<commit_message>
done with all test cases
</commit_message>
<xml_diff>
--- a/GUISeleniumFramework/testdata/testScriptdata.xlsx
+++ b/GUISeleniumFramework/testdata/testScriptdata.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\git\Dolibarr_GUIFramework1\GUISeleniumFramework\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA3DBEC-C8A9-41CC-B841-7F8A900E2473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11625" windowHeight="6330"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ThirdParty" sheetId="3" r:id="rId1"/>
@@ -14,8 +20,8 @@
     <sheet name="MRP" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="176">
   <si>
     <t>TC_ID</t>
   </si>
@@ -419,13 +425,183 @@
   </si>
   <si>
     <t>tc_02</t>
+  </si>
+  <si>
+    <t>TestCaseNames</t>
+  </si>
+  <si>
+    <t>TC_13</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CreateUserandGroupandVerifyForSalesTest</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Groupname</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>VerifySales_</t>
+  </si>
+  <si>
+    <t>Sale of product_</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Sales Executive</t>
+  </si>
+  <si>
+    <t>Jobposition</t>
+  </si>
+  <si>
+    <t>sahoo1234</t>
+  </si>
+  <si>
+    <t>Debipriya@12345</t>
+  </si>
+  <si>
+    <t>VerifyStocks_</t>
+  </si>
+  <si>
+    <t>Stocks of product_</t>
+  </si>
+  <si>
+    <t>sahoo1000</t>
+  </si>
+  <si>
+    <t>Debipriya@10000</t>
+  </si>
+  <si>
+    <t>Stocks Executive</t>
+  </si>
+  <si>
+    <t>TC_14</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CreateUserandGroupandVerifyForStocksTest</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>TC_15</t>
+  </si>
+  <si>
+    <t>Production_</t>
+  </si>
+  <si>
+    <t>Production department_</t>
+  </si>
+  <si>
+    <t>sahoo1001</t>
+  </si>
+  <si>
+    <t>Debipriya@10001</t>
+  </si>
+  <si>
+    <t>Production Executive</t>
+  </si>
+  <si>
+    <t>CreateUserandGroupForProductionTest</t>
+  </si>
+  <si>
+    <t>CreateNewBillOfMaterialForMRPTest- New Product page</t>
+  </si>
+  <si>
+    <t>Product ref.</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Oil manufacturing</t>
+  </si>
+  <si>
+    <t>CreateNewBillOfMaterialForMRPTest- New bill of materials</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>100'</t>
+  </si>
+  <si>
+    <t>10'</t>
+  </si>
+  <si>
+    <t>MRP3</t>
+  </si>
+  <si>
+    <t>HairOils_</t>
+  </si>
+  <si>
+    <t>CreateNewManufacturingOrderForMRPTest- New Manufacturing Order</t>
+  </si>
+  <si>
+    <t>Qty to produce</t>
+  </si>
+  <si>
+    <t>DateStartPlanned</t>
+  </si>
+  <si>
+    <t>DateEndPlanned</t>
+  </si>
+  <si>
+    <t>05/29/2024'</t>
+  </si>
+  <si>
+    <t>05/31/2024'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -450,8 +626,31 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -470,8 +669,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -505,30 +710,90 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -799,205 +1064,203 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="12" customWidth="1"/>
-    <col min="8" max="10" width="9.140625" style="12"/>
-    <col min="11" max="11" width="29.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="14.1796875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="30.81640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.54296875" style="9" customWidth="1"/>
+    <col min="8" max="10" width="9.1796875" style="9"/>
+    <col min="11" max="11" width="29.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.1796875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="6" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="11" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="6" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="11" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="11" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="13"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1006,123 +1269,57 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.81640625" customWidth="1"/>
+    <col min="3" max="3" width="18.26953125" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D2" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D5" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D8" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D11" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1130,55 +1327,129 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.36328125" customWidth="1"/>
+    <col min="3" max="3" width="11.90625" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" customWidth="1"/>
+    <col min="7" max="7" width="16.6328125" customWidth="1"/>
+    <col min="8" max="8" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2">
+    <row r="1" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{E311FF25-0AB8-4608-9323-5F649FACD3E0}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{621E51F9-A8A7-410F-9F49-3A863549FDF7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B100"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1186,7 +1457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1194,7 +1465,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1202,7 +1473,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1210,7 +1481,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1218,7 +1489,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1226,7 +1497,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1234,7 +1505,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1242,7 +1513,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1250,7 +1521,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -1258,7 +1529,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1266,7 +1537,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -1274,7 +1545,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -1282,7 +1553,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1290,7 +1561,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1298,7 +1569,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -1306,7 +1577,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
@@ -1314,7 +1585,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
@@ -1322,7 +1593,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>12</v>
       </c>
@@ -1330,7 +1601,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
@@ -1338,7 +1609,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>12</v>
       </c>
@@ -1346,7 +1617,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
@@ -1354,7 +1625,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>12</v>
       </c>
@@ -1362,7 +1633,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
@@ -1370,7 +1641,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
@@ -1378,7 +1649,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
@@ -1386,7 +1657,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>12</v>
       </c>
@@ -1394,7 +1665,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>12</v>
       </c>
@@ -1402,7 +1673,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>12</v>
       </c>
@@ -1410,7 +1681,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>12</v>
       </c>
@@ -1418,7 +1689,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>12</v>
       </c>
@@ -1426,7 +1697,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>12</v>
       </c>
@@ -1434,7 +1705,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>12</v>
       </c>
@@ -1442,7 +1713,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>12</v>
       </c>
@@ -1450,7 +1721,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>12</v>
       </c>
@@ -1458,7 +1729,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>12</v>
       </c>
@@ -1466,7 +1737,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>12</v>
       </c>
@@ -1474,7 +1745,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>12</v>
       </c>
@@ -1482,7 +1753,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>12</v>
       </c>
@@ -1490,7 +1761,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>12</v>
       </c>
@@ -1498,7 +1769,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>12</v>
       </c>
@@ -1506,7 +1777,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>12</v>
       </c>
@@ -1514,7 +1785,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>12</v>
       </c>
@@ -1522,7 +1793,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>12</v>
       </c>
@@ -1530,7 +1801,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>12</v>
       </c>
@@ -1538,7 +1809,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>12</v>
       </c>
@@ -1546,7 +1817,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>12</v>
       </c>
@@ -1554,7 +1825,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>12</v>
       </c>
@@ -1562,7 +1833,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>12</v>
       </c>
@@ -1570,7 +1841,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>12</v>
       </c>
@@ -1578,7 +1849,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>56</v>
       </c>
@@ -1586,7 +1857,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>56</v>
       </c>
@@ -1594,7 +1865,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>56</v>
       </c>
@@ -1602,7 +1873,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>56</v>
       </c>
@@ -1610,7 +1881,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>56</v>
       </c>
@@ -1618,7 +1889,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>56</v>
       </c>
@@ -1626,7 +1897,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
         <v>56</v>
       </c>
@@ -1634,7 +1905,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
         <v>56</v>
       </c>
@@ -1642,7 +1913,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
         <v>56</v>
       </c>
@@ -1650,7 +1921,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>56</v>
       </c>
@@ -1658,7 +1929,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>56</v>
       </c>
@@ -1666,7 +1937,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
         <v>56</v>
       </c>
@@ -1674,7 +1945,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
         <v>56</v>
       </c>
@@ -1682,7 +1953,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
         <v>56</v>
       </c>
@@ -1690,7 +1961,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>56</v>
       </c>
@@ -1698,7 +1969,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
         <v>56</v>
       </c>
@@ -1706,7 +1977,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
         <v>56</v>
       </c>
@@ -1714,7 +1985,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
         <v>56</v>
       </c>
@@ -1722,7 +1993,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
         <v>56</v>
       </c>
@@ -1730,7 +2001,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
         <v>56</v>
       </c>
@@ -1738,7 +2009,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
         <v>56</v>
       </c>
@@ -1746,7 +2017,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
         <v>56</v>
       </c>
@@ -1754,7 +2025,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
         <v>56</v>
       </c>
@@ -1762,7 +2033,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
         <v>56</v>
       </c>
@@ -1770,7 +2041,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>56</v>
       </c>
@@ -1778,7 +2049,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
         <v>56</v>
       </c>
@@ -1786,7 +2057,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
         <v>56</v>
       </c>
@@ -1794,7 +2065,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
         <v>56</v>
       </c>
@@ -1802,7 +2073,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
         <v>56</v>
       </c>
@@ -1810,7 +2081,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
         <v>56</v>
       </c>
@@ -1818,7 +2089,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
         <v>56</v>
       </c>
@@ -1826,7 +2097,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
         <v>56</v>
       </c>
@@ -1834,7 +2105,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
         <v>56</v>
       </c>
@@ -1842,7 +2113,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
         <v>56</v>
       </c>
@@ -1850,7 +2121,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
         <v>56</v>
       </c>
@@ -1858,7 +2129,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
         <v>56</v>
       </c>
@@ -1866,7 +2137,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
         <v>56</v>
       </c>
@@ -1874,7 +2145,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
         <v>56</v>
       </c>
@@ -1882,7 +2153,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
         <v>56</v>
       </c>
@@ -1890,7 +2161,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
         <v>56</v>
       </c>
@@ -1898,7 +2169,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
         <v>56</v>
       </c>
@@ -1906,7 +2177,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
         <v>56</v>
       </c>
@@ -1914,7 +2185,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
         <v>56</v>
       </c>
@@ -1922,7 +2193,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
         <v>56</v>
       </c>
@@ -1930,7 +2201,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
         <v>56</v>
       </c>
@@ -1938,7 +2209,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
         <v>56</v>
       </c>
@@ -1946,7 +2217,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
         <v>56</v>
       </c>
@@ -1954,7 +2225,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
         <v>56</v>
       </c>
@@ -1962,7 +2233,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
         <v>56</v>
       </c>
@@ -1970,7 +2241,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
         <v>56</v>
       </c>
@@ -1984,15 +2255,191 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="29.453125" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="17.1796875" customWidth="1"/>
+    <col min="6" max="6" width="13.6328125" customWidth="1"/>
+    <col min="7" max="7" width="17.90625" customWidth="1"/>
+    <col min="8" max="8" width="14.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="25" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="25" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+    </row>
+    <row r="5" spans="1:8" ht="24.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="25" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+    </row>
+    <row r="7" spans="1:8" ht="24.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="25" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+    </row>
+    <row r="9" spans="1:8" ht="24.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{F93D3F6D-79C9-4157-9AAE-231FAA1D26C7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>